<commit_message>
Add lake and river polygons to map
</commit_message>
<xml_diff>
--- a/SCChumStudy/DataIn/wild_ISC_chum_recruitment_PieterVanWill.xlsx
+++ b/SCChumStudy/DataIn/wild_ISC_chum_recruitment_PieterVanWill.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MDriveMyDocuments\Chum\2020\Data for Carrie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\SalmonLRP_RetroEval\SCChumStudy\DataIn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="100" yWindow="70" windowWidth="22850" windowHeight="12260"/>
+    <workbookView xWindow="105" yWindow="75" windowWidth="22845" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="UpdatedWild(Feb242021)" sheetId="2" r:id="rId1"/>
@@ -1580,50 +1580,50 @@
   <dimension ref="A1:BP102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="D3" activeCellId="1" sqref="D23 D3"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="23" width="13" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="13" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="13" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="35" max="36" width="13" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="13" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="40" max="44" width="13" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="13" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="49" max="50" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="51" max="55" width="13" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="57" max="59" width="13" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="61" max="67" width="13" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1695,7 +1695,7 @@
       <c r="BO1" s="16"/>
       <c r="BP1" s="16"/>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>34</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>1750.400120066005</v>
       </c>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>407.14627775873601</v>
       </c>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>55.249349875316199</v>
       </c>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>5</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>3082.7689371718402</v>
       </c>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>1638.61111631786</v>
       </c>
     </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
@@ -3137,7 +3137,7 @@
         <v>7930.9822554226103</v>
       </c>
     </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>24100.9112985395</v>
       </c>
     </row>
-    <row r="10" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>8035.1339012424205</v>
       </c>
     </row>
-    <row r="11" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>8</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>84806.671250989792</v>
       </c>
     </row>
-    <row r="12" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>8</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>25398.629817847323</v>
       </c>
     </row>
-    <row r="13" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>8</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>12936.285417443085</v>
       </c>
     </row>
-    <row r="14" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>8</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>164600.95681312957</v>
       </c>
     </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>8</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>184567.29358966861</v>
       </c>
     </row>
-    <row r="16" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>8</v>
       </c>
@@ -4785,7 +4785,7 @@
         <v>60764.56873931241</v>
       </c>
     </row>
-    <row r="17" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>8</v>
       </c>
@@ -4991,7 +4991,7 @@
         <v>836.37937412638166</v>
       </c>
     </row>
-    <row r="18" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>35</v>
       </c>
@@ -5197,7 +5197,7 @@
         <v>114606.219846657</v>
       </c>
     </row>
-    <row r="19" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>35</v>
       </c>
@@ -5403,7 +5403,7 @@
         <v>3651.4170886470201</v>
       </c>
     </row>
-    <row r="20" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>699169.62519421556</v>
       </c>
     </row>
-    <row r="22" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
@@ -5879,7 +5879,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="23" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>1</v>
       </c>
@@ -6085,7 +6085,7 @@
         <v>24.757736498130726</v>
       </c>
     </row>
-    <row r="24" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>3</v>
       </c>
@@ -6291,7 +6291,7 @@
         <v>5.758694909461858</v>
       </c>
     </row>
-    <row r="25" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>3</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>3.073773533039156</v>
       </c>
     </row>
-    <row r="26" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
         <v>5</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>72.671366350459465</v>
       </c>
     </row>
-    <row r="27" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
         <v>6</v>
       </c>
@@ -6909,7 +6909,7 @@
         <v>77.255292995858284</v>
       </c>
     </row>
-    <row r="28" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
         <v>6</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>486.1142145687412</v>
       </c>
     </row>
-    <row r="29" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
         <v>7</v>
       </c>
@@ -7321,7 +7321,7 @@
         <v>1613.5937577111724</v>
       </c>
     </row>
-    <row r="30" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>8</v>
       </c>
@@ -7527,7 +7527,7 @@
         <v>606.16501548827716</v>
       </c>
     </row>
-    <row r="31" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
         <v>8</v>
       </c>
@@ -7733,7 +7733,7 @@
         <v>6398.5570968684706</v>
       </c>
     </row>
-    <row r="32" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>8</v>
       </c>
@@ -7939,7 +7939,7 @@
         <v>2697.6499254726564</v>
       </c>
     </row>
-    <row r="33" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>8</v>
       </c>
@@ -8145,7 +8145,7 @@
         <v>975.33666749573388</v>
       </c>
     </row>
-    <row r="34" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
         <v>8</v>
       </c>
@@ -8351,7 +8351,7 @@
         <v>86086.683409086065</v>
       </c>
     </row>
-    <row r="35" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>8</v>
       </c>
@@ -8557,7 +8557,7 @@
         <v>50408.168756707128</v>
       </c>
     </row>
-    <row r="36" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>8</v>
       </c>
@@ -8763,7 +8763,7 @@
         <v>19352.961140450156</v>
       </c>
     </row>
-    <row r="37" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>8</v>
       </c>
@@ -8969,7 +8969,7 @@
         <v>235.66839502002671</v>
       </c>
     </row>
-    <row r="38" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
         <v>35</v>
       </c>
@@ -9175,7 +9175,7 @@
         <v>13997.465166855927</v>
       </c>
     </row>
-    <row r="39" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
         <v>35</v>
       </c>
@@ -9381,7 +9381,7 @@
         <v>275.30012364104743</v>
       </c>
     </row>
-    <row r="40" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>19</v>
       </c>
@@ -9648,7 +9648,7 @@
         <v>183317.18053365234</v>
       </c>
     </row>
-    <row r="42" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>20</v>
       </c>
@@ -9720,7 +9720,7 @@
       <c r="BO42" s="14"/>
       <c r="BP42" s="14"/>
     </row>
-    <row r="43" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>34</v>
       </c>
@@ -9926,7 +9926,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="44" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>1</v>
       </c>
@@ -10132,7 +10132,7 @@
         <v>1775.1578565641357</v>
       </c>
     </row>
-    <row r="45" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>3</v>
       </c>
@@ -10338,7 +10338,7 @@
         <v>412.90497266819784</v>
       </c>
     </row>
-    <row r="46" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>3</v>
       </c>
@@ -10544,7 +10544,7 @@
         <v>58.323123408355357</v>
       </c>
     </row>
-    <row r="47" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>5</v>
       </c>
@@ -10750,7 +10750,7 @@
         <v>3155.4403035222995</v>
       </c>
     </row>
-    <row r="48" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>6</v>
       </c>
@@ -10956,7 +10956,7 @@
         <v>1715.8664093137183</v>
       </c>
     </row>
-    <row r="49" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>6</v>
       </c>
@@ -11162,7 +11162,7 @@
         <v>8417.0964699913511</v>
       </c>
     </row>
-    <row r="50" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>7</v>
       </c>
@@ -11368,7 +11368,7 @@
         <v>25714.505056250673</v>
       </c>
     </row>
-    <row r="51" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>8</v>
       </c>
@@ -11574,7 +11574,7 @@
         <v>8641.2989167306969</v>
       </c>
     </row>
-    <row r="52" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>8</v>
       </c>
@@ -11780,7 +11780,7 @@
         <v>91205.228347858269</v>
       </c>
     </row>
-    <row r="53" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>8</v>
       </c>
@@ -11986,7 +11986,7 @@
         <v>28096.279743319978</v>
       </c>
     </row>
-    <row r="54" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>8</v>
       </c>
@@ -12192,7 +12192,7 @@
         <v>13911.622084938819</v>
       </c>
     </row>
-    <row r="55" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>8</v>
       </c>
@@ -12398,7 +12398,7 @@
         <v>250687.64022221562</v>
       </c>
     </row>
-    <row r="56" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>8</v>
       </c>
@@ -12604,7 +12604,7 @@
         <v>234975.46234637575</v>
       </c>
     </row>
-    <row r="57" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>8</v>
       </c>
@@ -12810,7 +12810,7 @@
         <v>80117.529879762558</v>
       </c>
     </row>
-    <row r="58" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>8</v>
       </c>
@@ -13016,7 +13016,7 @@
         <v>1072.0477691464084</v>
       </c>
     </row>
-    <row r="59" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>35</v>
       </c>
@@ -13222,7 +13222,7 @@
         <v>128603.68501351292</v>
       </c>
     </row>
-    <row r="60" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>35</v>
       </c>
@@ -13428,7 +13428,7 @@
         <v>3926.7172122880675</v>
       </c>
     </row>
-    <row r="61" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>21</v>
       </c>
@@ -13695,12 +13695,12 @@
         <v>882486.80572786776</v>
       </c>
     </row>
-    <row r="63" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>23</v>
       </c>
@@ -13906,7 +13906,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="65" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>25</v>
       </c>
@@ -14112,7 +14112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
         <v>26</v>
       </c>
@@ -14318,7 +14318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
         <v>26</v>
       </c>
@@ -14524,7 +14524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A68" s="8" t="s">
         <v>27</v>
       </c>
@@ -14730,7 +14730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A69" s="8" t="s">
         <v>28</v>
       </c>
@@ -14936,7 +14936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A70" s="8" t="s">
         <v>28</v>
       </c>
@@ -15142,7 +15142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>29</v>
       </c>
@@ -15348,7 +15348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>30</v>
       </c>
@@ -15554,7 +15554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>30</v>
       </c>
@@ -15760,7 +15760,7 @@
         <v>0.32751239241879193</v>
       </c>
     </row>
-    <row r="74" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
         <v>30</v>
       </c>
@@ -15966,7 +15966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A75" s="8" t="s">
         <v>30</v>
       </c>
@@ -16172,7 +16172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>30</v>
       </c>
@@ -16378,7 +16378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>30</v>
       </c>
@@ -16584,7 +16584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>30</v>
       </c>
@@ -16790,7 +16790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>30</v>
       </c>
@@ -16996,7 +16996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
         <v>31</v>
       </c>
@@ -17202,7 +17202,7 @@
         <v>0.98357539129591132</v>
       </c>
     </row>
-    <row r="81" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
         <v>31</v>
       </c>
@@ -17408,7 +17408,7 @@
         <v>0.98154968303191381</v>
       </c>
     </row>
-    <row r="83" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>32</v>
       </c>
@@ -17480,7 +17480,7 @@
       <c r="BO83" s="10"/>
       <c r="BP83" s="10"/>
     </row>
-    <row r="84" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="s">
         <v>23</v>
       </c>
@@ -17684,7 +17684,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="85" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="s">
         <v>25</v>
       </c>
@@ -17956,7 +17956,7 @@
         <v>1775.1578565641357</v>
       </c>
     </row>
-    <row r="86" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="s">
         <v>26</v>
       </c>
@@ -18228,7 +18228,7 @@
         <v>412.90497266819784</v>
       </c>
     </row>
-    <row r="87" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
         <v>26</v>
       </c>
@@ -18336,7 +18336,7 @@
         <v>1048.8877851124837</v>
       </c>
       <c r="AB87" s="23">
-        <f t="shared" ref="AB87:AI87" si="10">AB67*AB46</f>
+        <f t="shared" ref="AB87" si="10">AB67*AB46</f>
         <v>923.78945003957244</v>
       </c>
       <c r="AC87" s="23">
@@ -18500,7 +18500,7 @@
         <v>58.323123408355357</v>
       </c>
     </row>
-    <row r="88" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="s">
         <v>27</v>
       </c>
@@ -18608,7 +18608,7 @@
         <v>1218.1597274214419</v>
       </c>
       <c r="AB88" s="23">
-        <f t="shared" ref="AB88:AI88" si="11">AB68*AB47</f>
+        <f t="shared" ref="AB88" si="11">AB68*AB47</f>
         <v>10128.988668541471</v>
       </c>
       <c r="AC88" s="23">
@@ -18772,7 +18772,7 @@
         <v>3155.4403035222995</v>
       </c>
     </row>
-    <row r="89" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="s">
         <v>28</v>
       </c>
@@ -18880,7 +18880,7 @@
         <v>2151.82063090772</v>
       </c>
       <c r="AB89" s="23">
-        <f t="shared" ref="AB89:AI89" si="12">AB69*AB48</f>
+        <f t="shared" ref="AB89" si="12">AB69*AB48</f>
         <v>3640.4738822826716</v>
       </c>
       <c r="AC89" s="23">
@@ -19044,7 +19044,7 @@
         <v>1715.8664093137183</v>
       </c>
     </row>
-    <row r="90" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="s">
         <v>28</v>
       </c>
@@ -19152,7 +19152,7 @@
         <v>35651.237340154352</v>
       </c>
       <c r="AB90" s="23">
-        <f t="shared" ref="AB90:AI90" si="13">AB70*AB49</f>
+        <f t="shared" ref="AB90" si="13">AB70*AB49</f>
         <v>26977.189565562618</v>
       </c>
       <c r="AC90" s="23">
@@ -19316,7 +19316,7 @@
         <v>8417.0964699913511</v>
       </c>
     </row>
-    <row r="91" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="s">
         <v>29</v>
       </c>
@@ -19424,7 +19424,7 @@
         <v>96576.595841414965</v>
       </c>
       <c r="AB91" s="23">
-        <f t="shared" ref="AB91:AI91" si="14">AB71*AB50</f>
+        <f t="shared" ref="AB91" si="14">AB71*AB50</f>
         <v>281641.51963836863</v>
       </c>
       <c r="AC91" s="23">
@@ -19588,7 +19588,7 @@
         <v>25714.505056250673</v>
       </c>
     </row>
-    <row r="92" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="s">
         <v>30</v>
       </c>
@@ -19696,7 +19696,7 @@
         <v>17709.374402746642</v>
       </c>
       <c r="AB92" s="23">
-        <f t="shared" ref="AB92:AI92" si="15">AB72*AB51</f>
+        <f t="shared" ref="AB92" si="15">AB72*AB51</f>
         <v>27949.537789226692</v>
       </c>
       <c r="AC92" s="23">
@@ -19860,7 +19860,7 @@
         <v>8641.2989167306969</v>
       </c>
     </row>
-    <row r="93" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
         <v>30</v>
       </c>
@@ -19968,7 +19968,7 @@
         <v>16508.510510416199</v>
       </c>
       <c r="AB93" s="23">
-        <f t="shared" ref="AB93:AI93" si="16">AB73*AB52</f>
+        <f t="shared" ref="AB93" si="16">AB73*AB52</f>
         <v>72949.80876876456</v>
       </c>
       <c r="AC93" s="23">
@@ -20132,7 +20132,7 @@
         <v>29870.842537309283</v>
       </c>
     </row>
-    <row r="94" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="s">
         <v>30</v>
       </c>
@@ -20240,7 +20240,7 @@
         <v>46676.351611589387</v>
       </c>
       <c r="AB94" s="23">
-        <f t="shared" ref="AB94:AI94" si="17">AB74*AB53</f>
+        <f t="shared" ref="AB94" si="17">AB74*AB53</f>
         <v>55087.539197100661</v>
       </c>
       <c r="AC94" s="23">
@@ -20404,7 +20404,7 @@
         <v>28096.279743319978</v>
       </c>
     </row>
-    <row r="95" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="s">
         <v>30</v>
       </c>
@@ -20512,7 +20512,7 @@
         <v>90220.913337483813</v>
       </c>
       <c r="AB95" s="23">
-        <f t="shared" ref="AB95:AI95" si="18">AB75*AB54</f>
+        <f t="shared" ref="AB95" si="18">AB75*AB54</f>
         <v>62356.964764616903</v>
       </c>
       <c r="AC95" s="23">
@@ -20676,7 +20676,7 @@
         <v>13911.622084938819</v>
       </c>
     </row>
-    <row r="96" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="s">
         <v>30</v>
       </c>
@@ -20784,7 +20784,7 @@
         <v>105560.43994582229</v>
       </c>
       <c r="AB96" s="23">
-        <f t="shared" ref="AB96:AI96" si="20">AB76*AB55</f>
+        <f t="shared" ref="AB96" si="20">AB76*AB55</f>
         <v>169641.56613809263</v>
       </c>
       <c r="AC96" s="23">
@@ -20948,7 +20948,7 @@
         <v>250687.64022221562</v>
       </c>
     </row>
-    <row r="97" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="s">
         <v>30</v>
       </c>
@@ -21220,7 +21220,7 @@
         <v>234975.46234637575</v>
       </c>
     </row>
-    <row r="98" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
         <v>30</v>
       </c>
@@ -21492,7 +21492,7 @@
         <v>80117.529879762558</v>
       </c>
     </row>
-    <row r="99" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
         <v>30</v>
       </c>
@@ -21764,7 +21764,7 @@
         <v>1072.0477691464084</v>
       </c>
     </row>
-    <row r="100" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A100" s="10" t="s">
         <v>31</v>
       </c>
@@ -22036,7 +22036,7 @@
         <v>126491.41980926209</v>
       </c>
     </row>
-    <row r="101" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="s">
         <v>31</v>
       </c>
@@ -22308,7 +22308,7 @@
         <v>3854.268035077313</v>
       </c>
     </row>
-    <row r="102" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A102" s="9"/>
       <c r="B102" s="9" t="s">
         <v>33</v>

</xml_diff>